<commit_message>
processor finished and isa changed for je,ja,jbe,jae,jb and jump. also assemblier achanged for them to correctly assembly the given instructions
</commit_message>
<xml_diff>
--- a/InstructionSet.xlsx
+++ b/InstructionSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerim\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerim\Desktop\processor-digital-logic-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111DB95A-7826-455A-9312-28BEB0F21805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC26C88-E08B-46DC-A744-45ADA3337F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{704F6ED9-1D9E-4A4F-97CC-A0BCB1A3E17A}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{704F6ED9-1D9E-4A4F-97CC-A0BCB1A3E17A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,9 +161,6 @@
     <t>OP2</t>
   </si>
   <si>
-    <t>PCoffset14</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>0000</t>
+  </si>
+  <si>
+    <t>ADDR11</t>
   </si>
 </sst>
 </file>
@@ -250,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -273,16 +273,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -601,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCC5834-B1C8-44BD-BF07-C1B81964CD18}">
   <dimension ref="B1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,10 +683,10 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="U2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -689,10 +735,10 @@
         <v>0</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -727,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V4" s="3" t="s">
         <v>18</v>
@@ -765,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>19</v>
@@ -803,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V6" s="3" t="s">
         <v>21</v>
@@ -841,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V7" s="3" t="s">
         <v>20</v>
@@ -875,7 +921,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="U8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>22</v>
@@ -909,7 +955,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="U9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V9" s="3" t="s">
         <v>23</v>
@@ -922,24 +968,30 @@
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="D10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
       <c r="U10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V10" s="3" t="s">
         <v>24</v>
@@ -971,7 +1023,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="U11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V11" s="3" t="s">
         <v>25</v>
@@ -1003,7 +1055,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="U12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V12" s="3" t="s">
         <v>26</v>
@@ -1047,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V13" s="3" t="s">
         <v>27</v>
@@ -1060,21 +1112,19 @@
       <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
+      <c r="D14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="7"/>
       <c r="O14" s="2">
         <v>0</v>
       </c>
@@ -1085,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V14" s="3" t="s">
         <v>28</v>
@@ -1098,21 +1148,19 @@
       <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="2">
-        <v>0</v>
-      </c>
+      <c r="D15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
       <c r="O15" s="2">
         <v>0</v>
       </c>
@@ -1123,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V15" s="3" t="s">
         <v>29</v>
@@ -1136,21 +1184,19 @@
       <c r="C16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="2">
-        <v>0</v>
-      </c>
+      <c r="D16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="7"/>
       <c r="O16" s="2">
         <v>0</v>
       </c>
@@ -1161,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V16" s="3" t="s">
         <v>30</v>
@@ -1174,21 +1220,19 @@
       <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="2">
-        <v>0</v>
-      </c>
+      <c r="D17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="7"/>
       <c r="O17" s="2">
         <v>0</v>
       </c>
@@ -1199,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V17" s="3" t="s">
         <v>31</v>
@@ -1212,21 +1256,19 @@
       <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
+      <c r="D18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="7"/>
       <c r="O18" s="2">
         <v>0</v>
       </c>
@@ -1237,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V18" s="3" t="s">
         <v>32</v>
@@ -1293,13 +1335,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="D14:N14"/>
+    <mergeCell ref="D15:N15"/>
+    <mergeCell ref="D16:N16"/>
+    <mergeCell ref="D17:N17"/>
+    <mergeCell ref="D18:N18"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H12:Q12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:Q9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:Q11"/>
+    <mergeCell ref="D10:N10"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="H7:K7"/>
@@ -1309,21 +1359,13 @@
     <mergeCell ref="L8:Q8"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:Q9"/>
-    <mergeCell ref="D10:Q10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:Q11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:Q12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="D14:M14"/>
-    <mergeCell ref="D15:M15"/>
-    <mergeCell ref="D16:M16"/>
-    <mergeCell ref="D17:M17"/>
-    <mergeCell ref="D18:M18"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="L5:O5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1332,15 +1374,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Belge" ma:contentTypeID="0x01010046AC7CD1758C8D489C39BCA61006E69E" ma:contentTypeVersion="2" ma:contentTypeDescription="Yeni belge oluşturun." ma:contentTypeScope="" ma:versionID="3d3b253070ad41928a00ad30207b864a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1a019847-6c66-47bb-a1bc-a252058d1315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1a275b445d18be14f535e0ca99bc60e" ns3:_="">
     <xsd:import namespace="1a019847-6c66-47bb-a1bc-a252058d1315"/>
@@ -1472,6 +1505,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1479,14 +1521,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10417B34-E40C-48F7-9954-293289C26C88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E6FDE79-429F-40F0-8C57-D0843236B8A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1500,6 +1534,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10417B34-E40C-48F7-9954-293289C26C88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>